<commit_message>
testing differernt file formats
</commit_message>
<xml_diff>
--- a/master_table.xlsx
+++ b/master_table.xlsx
@@ -3422,11 +3422,11 @@
   <dimension ref="A1:AMJ144"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B99" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A99" activeCellId="0" sqref="A99"/>
+      <selection pane="bottomRight" activeCell="D105" activeCellId="0" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11571,7 +11571,7 @@
         <v>498</v>
       </c>
       <c r="B105" s="19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C105" s="18" t="s">
         <v>24</v>
@@ -11646,7 +11646,7 @@
         <v>507</v>
       </c>
       <c r="B106" s="14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C106" s="13" t="s">
         <v>24</v>
@@ -14088,7 +14088,7 @@
         <v>624</v>
       </c>
       <c r="B137" s="96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C137" s="95" t="s">
         <v>210</v>

</xml_diff>